<commit_message>
Added calculations to determine maximum uart to rf bridge rx timer interval.
</commit_message>
<xml_diff>
--- a/Engineering_Documents/timer_Calculations.xlsx
+++ b/Engineering_Documents/timer_Calculations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brent\git\kb1lqd\faradayio-firmware\Engineering_Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\faraday_git\faradayio-firmware\Engineering_Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="7260" xr2:uid="{FC6F9794-1E28-4DD8-9A84-9165D86BA3C1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="7260" xr2:uid="{FC6F9794-1E28-4DD8-9A84-9165D86BA3C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Timers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>fmclk</t>
   </si>
@@ -63,13 +63,49 @@
   </si>
   <si>
     <t>Hz</t>
+  </si>
+  <si>
+    <t>Timer A CCR2 (Uart To RF Bridge RX Timer)</t>
+  </si>
+  <si>
+    <t>UART Baudrate</t>
+  </si>
+  <si>
+    <t>RF Baudrate</t>
+  </si>
+  <si>
+    <t>Baud</t>
+  </si>
+  <si>
+    <t>UART Bit Period</t>
+  </si>
+  <si>
+    <t>RF Bit Period</t>
+  </si>
+  <si>
+    <t>RF Packet Size</t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t>RF Packet Duration</t>
+  </si>
+  <si>
+    <t>UART Buffer Size</t>
+  </si>
+  <si>
+    <t>UART Max Timer Duration</t>
+  </si>
+  <si>
+    <t>Minimum Time Interval</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +124,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -201,6 +245,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -208,7 +261,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
@@ -243,6 +296,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -581,25 +643,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDD8497-3673-468D-9E81-0DB48C223D61}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -610,7 +672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -621,7 +683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -632,15 +694,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
@@ -651,7 +713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -662,7 +724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -674,15 +736,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -693,7 +755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -704,7 +766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -716,10 +778,159 @@
         <v>11</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5">
+        <v>115200</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="15">
+        <f>1/B17</f>
+        <v>8.6805555555555555E-6</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="5">
+        <v>255</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="15">
+        <f>B19*B18</f>
+        <v>2.2135416666666666E-3</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="5">
+        <v>38383.483999999997</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="15">
+        <f>1/B21</f>
+        <v>2.6052872115517187E-5</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="5">
+        <v>255</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="15">
+        <f>B23*B22</f>
+        <v>6.6434823894568826E-3</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15">
+        <f>MIN(B20,B24)</f>
+        <v>2.2135416666666666E-3</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="12">
+        <f>ROUND(B28*B8,0)</f>
+        <v>312</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A15:C15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>